<commit_message>
corrected typo in sprint 2 burndown chart
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint 2/Burndown Chart.xlsx
+++ b/Project/Phase 2/Sprint 2/Burndown Chart.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accga\OneDrive\Desktop\uni\Year 3\Sem 1\Engenharia de Software\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CA69CE2-55A7-4D33-80AB-D07E03135945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F825261C-25FD-4294-9820-A19697DC7066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 3" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -179,14 +179,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -260,7 +260,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 3'!$A$3:$A$9</c:f>
+              <c:f>'Sprint 2'!$A$3:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -290,7 +290,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 3'!$B$3:$B$9</c:f>
+              <c:f>'Sprint 2'!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -340,7 +340,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sprint 3'!$A$3:$A$9</c:f>
+              <c:f>'Sprint 2'!$A$3:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -370,7 +370,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 3'!$C$3:$C$9</c:f>
+              <c:f>'Sprint 2'!$C$3:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -840,11 +840,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -931,13 +931,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <v>0.5</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>4</v>
       </c>
     </row>

</xml_diff>